<commit_message>
test automation chuc nang tim kiem va gio hang
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Đăng nhập" sheetId="1" r:id="rId1"/>
-    <sheet name="Đăng kí" sheetId="2" r:id="rId2"/>
+    <sheet name="Giỏ hàng" sheetId="4" r:id="rId2"/>
+    <sheet name="Tìm kiếm" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>0348340873</t>
   </si>
@@ -33,15 +34,9 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Username(Email hoặc Sđt)</t>
-  </si>
-  <si>
     <t>thanhlevt7@gmail.com</t>
   </si>
   <si>
-    <t>thanhlevt7</t>
-  </si>
-  <si>
     <t>123456</t>
   </si>
   <si>
@@ -52,13 +47,31 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>rau</t>
+  </si>
+  <si>
+    <t>@@@</t>
+  </si>
+  <si>
+    <t>Từ khóa tìm kiếm</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>!@#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +82,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -98,10 +119,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -383,41 +406,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>123456789</v>
       </c>
@@ -425,76 +448,39 @@
         <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
         <v>123</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>123</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1234</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1">
-        <v>123</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>1234</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="thanhlevt7@gmail.com"/>
-    <hyperlink ref="A7" r:id="rId2"/>
-    <hyperlink ref="A6" r:id="rId3" display="thanhlevt7@gmail.com"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -502,25 +488,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>